<commit_message>
updating analysis and creating jif/second code
</commit_message>
<xml_diff>
--- a/analysis/coded_responses.xlsx
+++ b/analysis/coded_responses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8703" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9501" uniqueCount="1157">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3392,6 +3392,96 @@
   </si>
   <si>
     <t>Glottochronology</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> e36ab195</t>
+  </si>
+  <si>
+    <t>Authors say that they are, but "minimally"</t>
+  </si>
+  <si>
+    <t>Public website</t>
+  </si>
+  <si>
+    <t>The corpus can be accessed freely (no data files)</t>
+  </si>
+  <si>
+    <t>English, Czech</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>cross lingusitics</t>
+  </si>
+  <si>
+    <t>Can't find</t>
+  </si>
+  <si>
+    <t>German, French, English</t>
+  </si>
+  <si>
+    <t>Some background poll data available from a third party</t>
+  </si>
+  <si>
+    <t>Aboriginal languages</t>
+  </si>
+  <si>
+    <t>In the Appendices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard and dialectal Arabic, French, and Ama- zigh (Berber) </t>
+  </si>
+  <si>
+    <t>Field study or language description, Survey or interview</t>
+  </si>
+  <si>
+    <t>Northern Samoyedic languages</t>
+  </si>
+  <si>
+    <t>Partial materials in the appendix</t>
+  </si>
+  <si>
+    <t>Not applicable?</t>
+  </si>
+  <si>
+    <t>Malysia</t>
+  </si>
+  <si>
+    <t>Discourse analysis?</t>
+  </si>
+  <si>
+    <t>Statement sats that the data will be available in the future when database is completed</t>
+  </si>
+  <si>
+    <t>Link to the corpus</t>
+  </si>
+  <si>
+    <t>Languages of Belize</t>
+  </si>
+  <si>
+    <t>English, Afrikaans</t>
+  </si>
+  <si>
+    <t>Link to one corpus</t>
+  </si>
+  <si>
+    <t>Dead link to the test application</t>
+  </si>
+  <si>
+    <t>No applicable</t>
+  </si>
+  <si>
+    <t>Some available through a third party</t>
+  </si>
+  <si>
+    <t>Corpus cited, other data not available</t>
+  </si>
+  <si>
+    <t>Some available in appendix</t>
+  </si>
+  <si>
+    <t>Some available in the appendix</t>
   </si>
 </sst>
 </file>
@@ -43307,8 +43397,3501 @@
         <v>71</v>
       </c>
     </row>
+    <row r="698">
+      <c r="A698" s="3">
+        <v>44644.399334918984</v>
+      </c>
+      <c r="B698" s="4">
+        <v>0.35347222222480923</v>
+      </c>
+      <c r="C698" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="D698" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E698" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F698" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G698" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H698" s="2">
+        <v>2.06</v>
+      </c>
+      <c r="I698" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J698" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N698" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O698" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S698" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W698" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z698" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA698" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB698" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC698" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD698" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF698" s="4">
+        <v>0.3569444444437977</v>
+      </c>
+      <c r="AG698" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="AH698" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="AJ698" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK698" s="2">
+        <v>2018.0</v>
+      </c>
+    </row>
     <row r="699">
-      <c r="AH699" s="6">
+      <c r="A699" s="3">
+        <v>44644.40273079861</v>
+      </c>
+      <c r="B699" s="4">
+        <v>0.36041666666278616</v>
+      </c>
+      <c r="C699" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="D699" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E699" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="F699" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF699" s="4">
+        <v>0.36041666666278616</v>
+      </c>
+      <c r="AG699" s="5">
+        <v>44644.0</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" s="3">
+        <v>44644.40966449074</v>
+      </c>
+      <c r="B700" s="4">
+        <v>0.36527777777519077</v>
+      </c>
+      <c r="C700" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="D700" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E700" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="F700" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G700" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="H700" s="2">
+        <v>3.02</v>
+      </c>
+      <c r="I700" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J700" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N700" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="O700" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="P700" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q700" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R700" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S700" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W700" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z700" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC700" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD700" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF700" s="4">
+        <v>0.367361111115315</v>
+      </c>
+      <c r="AG700" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="AH700" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AJ700" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK700" s="2">
+        <v>2019.0</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" s="3">
+        <v>44644.414326412036</v>
+      </c>
+      <c r="B701" s="4">
+        <v>0.3694444444408873</v>
+      </c>
+      <c r="C701" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="D701" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E701" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="F701" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G701" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="H701" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="I701" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC701" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF701" s="4">
+        <v>0.37222222222044365</v>
+      </c>
+      <c r="AG701" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="AH701" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK701" s="2">
+        <v>2019.0</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" s="3">
+        <v>44644.416295069444</v>
+      </c>
+      <c r="B702" s="4">
+        <v>0.37291666666715173</v>
+      </c>
+      <c r="C702" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="D702" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E702" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F702" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G702" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="H702" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="I702" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC702" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF702" s="4">
+        <v>0.3743055555532919</v>
+      </c>
+      <c r="AG702" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="AH702" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK702" s="2">
+        <v>2019.0</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" s="3">
+        <v>44644.88225328704</v>
+      </c>
+      <c r="B703" s="4">
+        <v>0.6729166666627862</v>
+      </c>
+      <c r="C703" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="D703" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E703" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F703" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G703" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="H703" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I703" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC703" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF703" s="4">
+        <v>0.6736111111094942</v>
+      </c>
+      <c r="AG703" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="AH703" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" s="3">
+        <v>44644.88553697917</v>
+      </c>
+      <c r="B704" s="4">
+        <v>0.6756944444423425</v>
+      </c>
+      <c r="C704" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="D704" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E704" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="F704" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G704" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H704" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I704" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J704" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N704" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="O704" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S704" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W704" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z704" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC704" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD704" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF704" s="4">
+        <v>0.6763888888890506</v>
+      </c>
+      <c r="AG704" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="AH704" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AJ704" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" s="3">
+        <v>44644.88893032407</v>
+      </c>
+      <c r="B705" s="4">
+        <v>0.6784722222218988</v>
+      </c>
+      <c r="C705" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="D705" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E705" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="F705" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G705" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H705" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I705" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J705" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N705" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="O705" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="P705" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q705" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R705" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="S705" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W705" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z705" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC705" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD705" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF705" s="4">
+        <v>0.679861111115315</v>
+      </c>
+      <c r="AG705" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="AH705" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ705" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" s="3">
+        <v>44645.09339594908</v>
+      </c>
+      <c r="B706" s="4">
+        <v>0.8833333333313931</v>
+      </c>
+      <c r="C706" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="D706" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E706" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F706" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G706" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H706" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I706" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J706" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N706" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O706" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="P706" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="Q706" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="R706" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S706" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W706" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z706" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC706" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD706" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF706" s="4">
+        <v>0.8847222222248092</v>
+      </c>
+      <c r="AG706" s="5">
+        <v>44644.0</v>
+      </c>
+      <c r="AH706" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AJ706" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" s="3">
+        <v>44645.329028078704</v>
+      </c>
+      <c r="B707" s="4">
+        <v>0.28402777777955635</v>
+      </c>
+      <c r="C707" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="D707" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E707" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F707" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G707" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="H707" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="I707" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J707" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N707" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="O707" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S707" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W707" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z707" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC707" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD707" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF707" s="4">
+        <v>0.2868055555591127</v>
+      </c>
+      <c r="AG707" s="5">
+        <v>45010.0</v>
+      </c>
+      <c r="AH707" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="AJ707" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK707" s="2">
+        <v>2017.0</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" s="3">
+        <v>44645.33457960648</v>
+      </c>
+      <c r="B708" s="4">
+        <v>0.29027777777810115</v>
+      </c>
+      <c r="C708" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="D708" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E708" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F708" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G708" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H708" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="I708" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J708" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N708" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O708" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S708" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W708" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z708" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC708" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD708" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF708" s="4">
+        <v>0.2923611111109494</v>
+      </c>
+      <c r="AG708" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="AH708" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AJ708" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK708" s="2">
+        <v>2019.0</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" s="3">
+        <v>44645.348867939814</v>
+      </c>
+      <c r="B709" s="4">
+        <v>0.3041666666686069</v>
+      </c>
+      <c r="C709" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="D709" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E709" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="F709" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G709" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H709" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I709" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="W709" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z709" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC709" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD709" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF709" s="4">
+        <v>0.3069444444408873</v>
+      </c>
+      <c r="AG709" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="AH709" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ709" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK709" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" s="3">
+        <v>44645.55691399306</v>
+      </c>
+      <c r="B710" s="4">
+        <v>0.5124999999970896</v>
+      </c>
+      <c r="C710" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="D710" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E710" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="F710" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G710" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H710" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="I710" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J710" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N710" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O710" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="P710" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q710" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R710" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S710" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W710" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z710" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC710" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD710" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF710" s="4">
+        <v>0.5145833333372138</v>
+      </c>
+      <c r="AG710" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="AH710" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="AJ710" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK710" s="2">
+        <v>2018.0</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" s="3">
+        <v>44645.55865761574</v>
+      </c>
+      <c r="B711" s="4">
+        <v>0.515972222223354</v>
+      </c>
+      <c r="C711" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="D711" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E711" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="F711" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF711" s="4">
+        <v>0.5166666666627862</v>
+      </c>
+      <c r="AG711" s="5">
+        <v>44645.0</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" s="3">
+        <v>44645.61359741898</v>
+      </c>
+      <c r="B712" s="4">
+        <v>0.40277777778101154</v>
+      </c>
+      <c r="C712" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="D712" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E712" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="F712" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G712" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="H712" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I712" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J712" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N712" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="O712" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S712" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W712" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z712" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC712" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD712" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF712" s="4">
+        <v>0.40486111110658385</v>
+      </c>
+      <c r="AG712" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="AH712" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AJ712" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" s="3">
+        <v>44645.61976918981</v>
+      </c>
+      <c r="B713" s="4">
+        <v>0.40902777777955635</v>
+      </c>
+      <c r="C713" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="D713" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E713" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="F713" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G713" s="2" t="s">
+        <v>1133</v>
+      </c>
+      <c r="H713" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I713" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J713" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N713" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="O713" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="P713" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q713" s="2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="R713" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="S713" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W713" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z713" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC713" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD713" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF713" s="4">
+        <v>0.4111111111124046</v>
+      </c>
+      <c r="AG713" s="5">
+        <v>44645.0</v>
+      </c>
+      <c r="AH713" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="AJ713" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" s="3">
+        <v>44646.67807141204</v>
+      </c>
+      <c r="B714" s="4">
+        <v>0.46875</v>
+      </c>
+      <c r="C714" s="5">
+        <v>44646.0</v>
+      </c>
+      <c r="D714" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E714" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F714" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G714" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H714" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I714" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J714" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N714" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="O714" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S714" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W714" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z714" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC714" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD714" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF714" s="4">
+        <v>0.4694444444467081</v>
+      </c>
+      <c r="AG714" s="5">
+        <v>44646.0</v>
+      </c>
+      <c r="AH714" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ714" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" s="3">
+        <v>44646.68117789352</v>
+      </c>
+      <c r="B715" s="4">
+        <v>0.47152777777955635</v>
+      </c>
+      <c r="C715" s="5">
+        <v>44646.0</v>
+      </c>
+      <c r="D715" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E715" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="F715" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G715" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H715" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I715" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J715" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N715" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O715" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S715" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W715" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z715" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC715" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD715" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF715" s="4">
+        <v>0.47222222221898846</v>
+      </c>
+      <c r="AG715" s="5">
+        <v>44646.0</v>
+      </c>
+      <c r="AH715" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ715" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" s="3">
+        <v>44646.682446736115</v>
+      </c>
+      <c r="B716" s="4">
+        <v>0.4736111111124046</v>
+      </c>
+      <c r="C716" s="5">
+        <v>44646.0</v>
+      </c>
+      <c r="D716" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E716" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="F716" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF716" s="4">
+        <v>0.4736111111124046</v>
+      </c>
+      <c r="AG716" s="5">
+        <v>44646.0</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" s="3">
+        <v>44646.68776688658</v>
+      </c>
+      <c r="B717" s="4">
+        <v>0.47777777777810115</v>
+      </c>
+      <c r="C717" s="5">
+        <v>44646.0</v>
+      </c>
+      <c r="D717" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E717" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="F717" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G717" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H717" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I717" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J717" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N717" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="O717" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="P717" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q717" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R717" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S717" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T717" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="U717" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V717" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W717" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z717" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC717" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD717" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF717" s="4">
+        <v>0.47916666666424135</v>
+      </c>
+      <c r="AG717" s="5">
+        <v>44646.0</v>
+      </c>
+      <c r="AH717" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AJ717" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" s="3">
+        <v>44648.44668947917</v>
+      </c>
+      <c r="B718" s="4">
+        <v>0.40277777778101154</v>
+      </c>
+      <c r="C718" s="5">
+        <v>44648.0</v>
+      </c>
+      <c r="D718" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E718" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="F718" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G718" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H718" s="2">
+        <v>1.77</v>
+      </c>
+      <c r="I718" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC718" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF718" s="4">
+        <v>0.40486111110658385</v>
+      </c>
+      <c r="AG718" s="5">
+        <v>44648.0</v>
+      </c>
+      <c r="AH718" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK718" s="2">
+        <v>2017.0</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" s="3">
+        <v>44648.451587881944</v>
+      </c>
+      <c r="B719" s="4">
+        <v>0.40625</v>
+      </c>
+      <c r="C719" s="5">
+        <v>44648.0</v>
+      </c>
+      <c r="D719" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E719" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F719" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G719" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H719" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="I719" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J719" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N719" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O719" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="P719" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q719" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R719" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S719" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W719" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z719" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC719" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD719" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF719" s="4">
+        <v>0.40972222221898846</v>
+      </c>
+      <c r="AG719" s="5">
+        <v>44648.0</v>
+      </c>
+      <c r="AH719" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AJ719" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK719" s="2">
+        <v>2019.0</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" s="3">
+        <v>44648.45883158565</v>
+      </c>
+      <c r="B720" s="4">
+        <v>0.4145833333313931</v>
+      </c>
+      <c r="C720" s="5">
+        <v>44648.0</v>
+      </c>
+      <c r="D720" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E720" s="2">
+        <v>9.8963718E7</v>
+      </c>
+      <c r="F720" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G720" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="H720" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="I720" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC720" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF720" s="4">
+        <v>0.41666666666424135</v>
+      </c>
+      <c r="AG720" s="5">
+        <v>44648.0</v>
+      </c>
+      <c r="AH720" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="AK720" s="2">
+        <v>2019.0</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" s="3">
+        <v>44649.42998215278</v>
+      </c>
+      <c r="B721" s="4">
+        <v>0.38541666666424135</v>
+      </c>
+      <c r="C721" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D721" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E721" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="F721" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G721" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="H721" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="I721" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC721" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF721" s="4">
+        <v>0.3874999999970896</v>
+      </c>
+      <c r="AG721" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH721" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK721" s="2">
+        <v>2018.0</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" s="3">
+        <v>44649.435628402774</v>
+      </c>
+      <c r="B722" s="4">
+        <v>0.38958333333721384</v>
+      </c>
+      <c r="C722" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D722" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E722" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F722" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G722" s="2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="H722" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I722" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J722" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N722" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O722" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S722" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W722" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z722" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA722" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB722" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC722" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD722" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF722" s="4">
+        <v>0.3937500000029104</v>
+      </c>
+      <c r="AG722" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH722" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AJ722" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK722" s="2">
+        <v>2022.0</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" s="3">
+        <v>44649.43999171296</v>
+      </c>
+      <c r="B723" s="4">
+        <v>0.39583333333575865</v>
+      </c>
+      <c r="C723" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D723" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E723" s="2" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F723" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G723" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H723" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I723" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J723" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N723" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O723" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S723" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W723" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z723" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC723" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD723" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF723" s="4">
+        <v>0.3979166666686069</v>
+      </c>
+      <c r="AG723" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH723" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ723" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK723" s="2">
+        <v>2019.0</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" s="3">
+        <v>44649.65484574074</v>
+      </c>
+      <c r="B724" s="4">
+        <v>0.6493055555547471</v>
+      </c>
+      <c r="C724" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D724" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E724" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F724" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G724" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H724" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I724" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J724" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N724" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O724" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S724" s="2" t="s">
+        <v>1136</v>
+      </c>
+      <c r="T724" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U724" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V724" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="W724" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z724" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC724" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD724" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF724" s="4">
+        <v>0.6541666666671517</v>
+      </c>
+      <c r="AG724" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH724" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ724" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" s="3">
+        <v>44649.659401157405</v>
+      </c>
+      <c r="B725" s="4">
+        <v>0.6555555555532919</v>
+      </c>
+      <c r="C725" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D725" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E725" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="F725" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G725" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H725" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I725" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J725" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N725" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="O725" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S725" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W725" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z725" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA725" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB725" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC725" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD725" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF725" s="4">
+        <v>0.6590277777795563</v>
+      </c>
+      <c r="AG725" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH725" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ725" s="2" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" s="3">
+        <v>44649.66180030092</v>
+      </c>
+      <c r="B726" s="4">
+        <v>0.6590277777795563</v>
+      </c>
+      <c r="C726" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D726" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E726" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="F726" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G726" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="H726" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I726" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC726" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF726" s="4">
+        <v>0.6611111111124046</v>
+      </c>
+      <c r="AG726" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH726" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" s="3">
+        <v>44649.66564125</v>
+      </c>
+      <c r="B727" s="4">
+        <v>0.6618055555591127</v>
+      </c>
+      <c r="C727" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D727" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E727" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="F727" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G727" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H727" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I727" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J727" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N727" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O727" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S727" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W727" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z727" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC727" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD727" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF727" s="4">
+        <v>0.6652777777781012</v>
+      </c>
+      <c r="AG727" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH727" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AJ727" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" s="3">
+        <v>44649.670300185186</v>
+      </c>
+      <c r="B728" s="4">
+        <v>0.6652777777781012</v>
+      </c>
+      <c r="C728" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D728" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E728" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F728" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G728" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H728" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I728" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J728" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N728" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="O728" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S728" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W728" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z728" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA728" s="2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="AB728" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC728" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD728" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF728" s="4">
+        <v>0.6701388888905058</v>
+      </c>
+      <c r="AG728" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH728" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ728" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" s="3">
+        <v>44649.67372928241</v>
+      </c>
+      <c r="B729" s="4">
+        <v>0.6701388888905058</v>
+      </c>
+      <c r="C729" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D729" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E729" s="2">
+        <v>8.6897574E7</v>
+      </c>
+      <c r="F729" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G729" s="2" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H729" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I729" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J729" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N729" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O729" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S729" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W729" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z729" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC729" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD729" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF729" s="4">
+        <v>0.6736111111094942</v>
+      </c>
+      <c r="AG729" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH729" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AJ729" s="2" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" s="3">
+        <v>44649.677998252315</v>
+      </c>
+      <c r="B730" s="4">
+        <v>0.6736111111094942</v>
+      </c>
+      <c r="C730" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D730" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E730" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F730" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G730" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H730" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I730" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J730" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N730" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O730" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S730" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W730" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z730" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC730" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD730" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF730" s="4">
+        <v>0.6777777777751908</v>
+      </c>
+      <c r="AG730" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH730" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AJ730" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" s="3">
+        <v>44649.78795596065</v>
+      </c>
+      <c r="B731" s="4">
+        <v>0.7833333333328483</v>
+      </c>
+      <c r="C731" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D731" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E731" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="F731" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G731" s="2" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H731" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="I731" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC731" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF731" s="4">
+        <v>0.7874999999985448</v>
+      </c>
+      <c r="AG731" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH731" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AK731" s="2">
+        <v>2011.0</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" s="3">
+        <v>44649.79775133102</v>
+      </c>
+      <c r="B732" s="4">
+        <v>0.7874999999985448</v>
+      </c>
+      <c r="C732" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D732" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E732" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="F732" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G732" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H732" s="2">
+        <v>1.297</v>
+      </c>
+      <c r="I732" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J732" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N732" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O732" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S732" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W732" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z732" s="2" t="s">
+        <v>1081</v>
+      </c>
+      <c r="AA732" s="2" t="s">
+        <v>1081</v>
+      </c>
+      <c r="AB732" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC732" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD732" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF732" s="4">
+        <v>0.797222222223354</v>
+      </c>
+      <c r="AG732" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH732" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AJ732" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK732" s="2">
+        <v>2010.0</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" s="3">
+        <v>44649.799999826384</v>
+      </c>
+      <c r="B733" s="4">
+        <v>0.7979166666627862</v>
+      </c>
+      <c r="C733" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D733" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E733" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F733" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G733" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H733" s="2">
+        <v>0.192</v>
+      </c>
+      <c r="I733" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC733" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF733" s="4">
+        <v>0.7993055555562023</v>
+      </c>
+      <c r="AG733" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH733" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK733" s="2">
+        <v>2013.0</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" s="3">
+        <v>44649.80311071759</v>
+      </c>
+      <c r="B734" s="4">
+        <v>0.8000000000029104</v>
+      </c>
+      <c r="C734" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D734" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E734" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F734" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G734" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H734" s="2">
+        <v>0.395</v>
+      </c>
+      <c r="I734" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC734" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF734" s="4">
+        <v>0.8027777777751908</v>
+      </c>
+      <c r="AG734" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH734" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK734" s="2">
+        <v>2009.0</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" s="3">
+        <v>44649.81394136574</v>
+      </c>
+      <c r="B735" s="4">
+        <v>0.8041666666686069</v>
+      </c>
+      <c r="C735" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D735" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E735" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F735" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G735" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H735" s="2">
+        <v>1.012</v>
+      </c>
+      <c r="I735" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J735" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N735" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O735" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S735" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W735" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z735" s="2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="AA735" s="2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="AB735" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC735" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD735" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF735" s="4">
+        <v>0.8131944444467081</v>
+      </c>
+      <c r="AG735" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH735" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ735" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK735" s="2">
+        <v>2010.0</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" s="3">
+        <v>44649.822147071754</v>
+      </c>
+      <c r="B736" s="4">
+        <v>0.8145833333328483</v>
+      </c>
+      <c r="C736" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D736" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E736" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="F736" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G736" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H736" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="I736" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J736" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N736" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O736" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S736" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W736" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z736" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC736" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD736" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF736" s="4">
+        <v>0.8215277777781012</v>
+      </c>
+      <c r="AG736" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH736" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="AJ736" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK736" s="2">
+        <v>2010.0</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" s="3">
+        <v>44649.825942615746</v>
+      </c>
+      <c r="B737" s="4">
+        <v>0.8222222222248092</v>
+      </c>
+      <c r="C737" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D737" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E737" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="F737" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G737" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H737" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="I737" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC737" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF737" s="4">
+        <v>0.8256944444437977</v>
+      </c>
+      <c r="AG737" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH737" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK737" s="2">
+        <v>2009.0</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" s="3">
+        <v>44649.83056206019</v>
+      </c>
+      <c r="B738" s="4">
+        <v>0.8256944444437977</v>
+      </c>
+      <c r="C738" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D738" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E738" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="F738" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G738" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H738" s="2">
+        <v>1.068</v>
+      </c>
+      <c r="I738" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J738" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N738" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O738" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="P738" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q738" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R738" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="S738" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W738" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z738" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC738" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD738" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF738" s="4">
+        <v>0.8298611111094942</v>
+      </c>
+      <c r="AG738" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH738" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ738" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK738" s="2">
+        <v>2010.0</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" s="3">
+        <v>44649.842291747686</v>
+      </c>
+      <c r="B739" s="4">
+        <v>0.8333333333357587</v>
+      </c>
+      <c r="C739" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D739" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E739" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="F739" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G739" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H739" s="2">
+        <v>1.526</v>
+      </c>
+      <c r="I739" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC739" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF739" s="4">
+        <v>0.8416666666671517</v>
+      </c>
+      <c r="AG739" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH739" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK739" s="2">
+        <v>2019.0</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" s="3">
+        <v>44649.85339984954</v>
+      </c>
+      <c r="B740" s="4">
+        <v>0.8486111111124046</v>
+      </c>
+      <c r="C740" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="D740" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E740" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="F740" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G740" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="H740" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I740" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J740" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N740" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="O740" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S740" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W740" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z740" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC740" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD740" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF740" s="4">
+        <v>0.8527777777781012</v>
+      </c>
+      <c r="AG740" s="5">
+        <v>44649.0</v>
+      </c>
+      <c r="AH740" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="AJ740" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" s="3">
+        <v>44651.68604136574</v>
+      </c>
+      <c r="B741" s="4">
+        <v>0.6812500000014552</v>
+      </c>
+      <c r="C741" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="D741" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E741" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="F741" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G741" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="H741" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I741" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J741" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N741" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O741" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S741" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W741" s="2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="Z741" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC741" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD741" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF741" s="4">
+        <v>0.6854166666671517</v>
+      </c>
+      <c r="AG741" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="AH741" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="AJ741" s="2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="AK741" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" s="3">
+        <v>44651.694476550925</v>
+      </c>
+      <c r="B742" s="4">
+        <v>0.6861111111065838</v>
+      </c>
+      <c r="C742" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="D742" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E742" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="F742" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G742" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="H742" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I742" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J742" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N742" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O742" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="P742" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="Q742" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="R742" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="S742" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="T742" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="U742" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="V742" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="W742" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z742" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC742" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD742" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF742" s="4">
+        <v>0.6937499999985448</v>
+      </c>
+      <c r="AG742" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="AH742" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="AJ742" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AK742" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" s="3">
+        <v>44651.70366291667</v>
+      </c>
+      <c r="B743" s="4">
+        <v>0.6965277777781012</v>
+      </c>
+      <c r="C743" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="D743" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E743" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="F743" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G743" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H743" s="2">
+        <v>1.596</v>
+      </c>
+      <c r="I743" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J743" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N743" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O743" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S743" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W743" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z743" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC743" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD743" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF743" s="4">
+        <v>0.703472222223354</v>
+      </c>
+      <c r="AG743" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="AH743" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AJ743" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK743" s="2">
+        <v>2020.0</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" s="3">
+        <v>44651.713438287035</v>
+      </c>
+      <c r="B744" s="4">
+        <v>0.7055555555562023</v>
+      </c>
+      <c r="C744" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="D744" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E744" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="F744" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G744" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="H744" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I744" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J744" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N744" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O744" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="P744" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="Q744" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R744" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="S744" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W744" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z744" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC744" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD744" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF744" s="4">
+        <v>0.7131944444408873</v>
+      </c>
+      <c r="AG744" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="AH744" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="AJ744" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK744" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" s="3">
+        <v>44651.71687556713</v>
+      </c>
+      <c r="B745" s="4">
+        <v>0.7131944444408873</v>
+      </c>
+      <c r="C745" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="D745" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E745" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="F745" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G745" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H745" s="2">
+        <v>1.292</v>
+      </c>
+      <c r="I745" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC745" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF745" s="4">
+        <v>0.7166666666671517</v>
+      </c>
+      <c r="AG745" s="5">
+        <v>44651.0</v>
+      </c>
+      <c r="AH745" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AK745" s="2">
+        <v>2019.0</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" s="3">
+        <v>44652.51909431713</v>
+      </c>
+      <c r="B746" s="4">
+        <v>0.5124999999970896</v>
+      </c>
+      <c r="C746" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="D746" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E746" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="F746" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G746" s="2" t="s">
+        <v>1149</v>
+      </c>
+      <c r="H746" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I746" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J746" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N746" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O746" s="2" t="s">
+        <v>1150</v>
+      </c>
+      <c r="P746" s="2" t="s">
+        <v>1150</v>
+      </c>
+      <c r="Q746" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R746" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="S746" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W746" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z746" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA746" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB746" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC746" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD746" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF746" s="4">
+        <v>0.5187500000029104</v>
+      </c>
+      <c r="AG746" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="AH746" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AJ746" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" s="3">
+        <v>44652.52478305556</v>
+      </c>
+      <c r="B747" s="4">
+        <v>0.5187500000029104</v>
+      </c>
+      <c r="C747" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="D747" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E747" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="F747" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G747" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="H747" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I747" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J747" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N747" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="O747" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S747" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W747" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z747" s="2" t="s">
+        <v>1151</v>
+      </c>
+      <c r="AA747" s="2" t="s">
+        <v>1151</v>
+      </c>
+      <c r="AB747" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC747" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD747" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF747" s="4">
+        <v>0.5243055555547471</v>
+      </c>
+      <c r="AG747" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="AH747" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="AJ747" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK747" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" s="3">
+        <v>44652.53179594908</v>
+      </c>
+      <c r="B748" s="4">
+        <v>0.5250000000014552</v>
+      </c>
+      <c r="C748" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="D748" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E748" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="F748" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G748" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="H748" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I748" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J748" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N748" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O748" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S748" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W748" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z748" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC748" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD748" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF748" s="4">
+        <v>0.53125</v>
+      </c>
+      <c r="AG748" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="AH748" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AJ748" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" s="3">
+        <v>44652.535625902776</v>
+      </c>
+      <c r="B749" s="4">
+        <v>0.5319444444467081</v>
+      </c>
+      <c r="C749" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="D749" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E749" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F749" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G749" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H749" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I749" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J749" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N749" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O749" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S749" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W749" s="2" t="s">
+        <v>1152</v>
+      </c>
+      <c r="Z749" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC749" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD749" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF749" s="4">
+        <v>0.5354166666656965</v>
+      </c>
+      <c r="AG749" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="AH749" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AJ749" s="2" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" s="3">
+        <v>44652.54021280093</v>
+      </c>
+      <c r="B750" s="4">
+        <v>0.5354166666656965</v>
+      </c>
+      <c r="C750" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="D750" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E750" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="F750" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G750" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H750" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I750" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J750" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N750" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O750" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S750" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W750" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z750" s="2" t="s">
+        <v>1153</v>
+      </c>
+      <c r="AA750" s="2" t="s">
+        <v>1153</v>
+      </c>
+      <c r="AB750" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC750" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD750" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF750" s="4">
+        <v>0.5395833333313931</v>
+      </c>
+      <c r="AG750" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="AH750" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ750" s="2" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" s="3">
+        <v>44652.54391947917</v>
+      </c>
+      <c r="B751" s="4">
+        <v>0.5402777777781012</v>
+      </c>
+      <c r="C751" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="D751" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E751" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="F751" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G751" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H751" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I751" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J751" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N751" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O751" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S751" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W751" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z751" s="2" t="s">
+        <v>1153</v>
+      </c>
+      <c r="AA751" s="2" t="s">
+        <v>1153</v>
+      </c>
+      <c r="AB751" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC751" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD751" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF751" s="4">
+        <v>0.5437499999970896</v>
+      </c>
+      <c r="AG751" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="AH751" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ751" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" s="3">
+        <v>44652.550977499995</v>
+      </c>
+      <c r="B752" s="4">
+        <v>0.5437499999970896</v>
+      </c>
+      <c r="C752" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="D752" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E752" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="F752" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G752" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H752" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I752" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J752" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N752" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O752" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="P752" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="Q752" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R752" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="S752" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W752" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z752" s="2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="AA752" s="2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="AB752" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC752" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD752" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF752" s="4">
+        <v>0.5506944444423425</v>
+      </c>
+      <c r="AG752" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="AH752" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ752" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" s="3">
+        <v>44652.55906945602</v>
+      </c>
+      <c r="B753" s="4">
+        <v>0.5513888888890506</v>
+      </c>
+      <c r="C753" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="D753" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E753" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F753" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G753" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H753" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I753" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J753" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N753" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O753" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S753" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="W753" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z753" s="2" t="s">
+        <v>1156</v>
+      </c>
+      <c r="AA753" s="2" t="s">
+        <v>1156</v>
+      </c>
+      <c r="AB753" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC753" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD753" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF753" s="4">
+        <v>0.5583333333343035</v>
+      </c>
+      <c r="AG753" s="5">
+        <v>44652.0</v>
+      </c>
+      <c r="AH753" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ753" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="AH755" s="6">
         <f>AVERAGE(AH2:AH32)</f>
         <v>0.007101254481</v>
       </c>

</xml_diff>